<commit_message>
time estimation, plotting to array, good measured2modelled
</commit_message>
<xml_diff>
--- a/input/sensors.xlsx
+++ b/input/sensors.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TRuStee\Deliverables\D3.3\retrieval\canopy_soil retrieval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TRuStee\Deliverables\D3.3\demonstrator\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="10380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="10380" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ASD" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="FLOX_full" localSheetId="2">FLOX_SPEC2!$A$1:$A$1025</definedName>
     <definedName name="sensor_1" localSheetId="1">HyPlant2018!$A$1:$B$627</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -520,7 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -5621,7 +5621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1025"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A1015" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
before flipping of .nc
</commit_message>
<xml_diff>
--- a/input/sensors.xlsx
+++ b/input/sensors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm_projects\demostrator\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAFD83F-44A8-450C-8EB2-C9BD35BE3CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7811F1-EF40-4039-8CCD-1997806C7855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASD" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Synergy" sheetId="13" r:id="rId8"/>
     <sheet name="MSI" sheetId="3" r:id="rId9"/>
     <sheet name="altum_multispec" sheetId="11" r:id="rId10"/>
+    <sheet name="george" sheetId="14" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="FLOX_full" localSheetId="2">FLOX_SPEC2!$A$1:$A$1025</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3879" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3891" uniqueCount="81">
   <si>
     <t>lambda</t>
   </si>
@@ -6976,12 +6977,137 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4B3A8E-D7C8-49E1-8EEA-0DF015378A39}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>475</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>550</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>560</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>660</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>668</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>717</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>735</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>790</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>840</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B627"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12015,7 +12141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1025"/>
   <sheetViews>
-    <sheetView topLeftCell="A952" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -32146,7 +32272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34353AF6-740A-4A58-AFE2-A843EFD95035}">
   <dimension ref="A1:BB244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BC1" sqref="BC1"/>
     </sheetView>
   </sheetViews>

</xml_diff>